<commit_message>
Add LinkedList Notes and Problems
</commit_message>
<xml_diff>
--- a/LEET_CODE_LIST.xlsx
+++ b/LEET_CODE_LIST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkat/Desktop/DSA_08_29_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D98D01C-8DD0-054D-8D61-E46DA5EFF1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75CA4BC5-E7AF-9F40-A98E-96209DC2036D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode Patterns" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'amazon 1M'!$A$1:$B$43</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Patterns'!$A$1:$G$127</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Patterns'!$A$1:$G$126</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'My Patterns'!$A$1:$F$233</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1254" uniqueCount="576">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="576">
   <si>
     <t>Problem Name</t>
   </si>
@@ -2331,13 +2331,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:X1002"/>
+  <dimension ref="A1:X1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F142" sqref="F142"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2382,7 +2382,7 @@
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
     </row>
-    <row r="2" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="D2" s="26"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
@@ -2412,7 +2412,7 @@
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
     </row>
-    <row r="3" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="26"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
@@ -2442,7 +2442,7 @@
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
     </row>
-    <row r="4" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -2450,7 +2450,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="26"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
@@ -2472,7 +2472,7 @@
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
     </row>
-    <row r="5" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>7</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="26"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -2502,7 +2502,7 @@
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
     </row>
-    <row r="6" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+      <c r="D6" s="26"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
@@ -2532,7 +2532,7 @@
       <c r="W6" s="3"/>
       <c r="X6" s="3"/>
     </row>
-    <row r="7" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
@@ -2540,7 +2540,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
@@ -2562,7 +2562,7 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -2570,7 +2570,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="26"/>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
@@ -2592,7 +2592,7 @@
       <c r="W8" s="3"/>
       <c r="X8" s="3"/>
     </row>
-    <row r="9" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="5" t="s">
         <v>13</v>
       </c>
@@ -2602,7 +2602,7 @@
       <c r="C9" s="3">
         <v>1</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="4"/>
@@ -2628,7 +2628,7 @@
       <c r="W9" s="3"/>
       <c r="X9" s="3"/>
     </row>
-    <row r="10" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
@@ -2638,7 +2638,7 @@
       <c r="C10" s="3">
         <v>1</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="D10" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E10" s="4"/>
@@ -2664,7 +2664,7 @@
       <c r="W10" s="3"/>
       <c r="X10" s="3"/>
     </row>
-    <row r="11" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A11" s="5" t="s">
         <v>17</v>
       </c>
@@ -2674,7 +2674,7 @@
       <c r="C11" s="3">
         <v>1</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="D11" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E11" s="4"/>
@@ -2700,7 +2700,7 @@
       <c r="W11" s="3"/>
       <c r="X11" s="3"/>
     </row>
-    <row r="12" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
         <v>18</v>
       </c>
@@ -2710,7 +2710,7 @@
       <c r="C12" s="3">
         <v>1</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E12" s="4"/>
@@ -2736,7 +2736,7 @@
       <c r="W12" s="3"/>
       <c r="X12" s="3"/>
     </row>
-    <row r="13" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
         <v>19</v>
       </c>
@@ -2746,7 +2746,7 @@
       <c r="C13" s="3">
         <v>1</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E13" s="4"/>
@@ -2770,7 +2770,7 @@
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
     </row>
-    <row r="14" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A14" s="5" t="s">
         <v>20</v>
       </c>
@@ -2780,7 +2780,7 @@
       <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="4"/>
@@ -2806,7 +2806,7 @@
       <c r="W14" s="3"/>
       <c r="X14" s="3"/>
     </row>
-    <row r="15" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A15" s="5" t="s">
         <v>568</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="3"/>
-      <c r="D15" s="4" t="s">
+      <c r="D15" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E15" s="3"/>
@@ -2838,7 +2838,7 @@
       <c r="W15" s="3"/>
       <c r="X15" s="3"/>
     </row>
-    <row r="16" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="5" t="s">
         <v>22</v>
       </c>
@@ -2848,7 +2848,7 @@
       <c r="C16" s="3">
         <v>1</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="D16" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="4"/>
@@ -2874,7 +2874,7 @@
       <c r="W16" s="3"/>
       <c r="X16" s="3"/>
     </row>
-    <row r="17" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="5" t="s">
         <v>23</v>
       </c>
@@ -2884,7 +2884,7 @@
       <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="4" t="s">
+      <c r="D17" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E17" s="4"/>
@@ -2910,7 +2910,7 @@
       <c r="W17" s="3"/>
       <c r="X17" s="3"/>
     </row>
-    <row r="18" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A18" s="6" t="s">
         <v>24</v>
       </c>
@@ -2920,7 +2920,7 @@
       <c r="C18" s="3">
         <v>1</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E18" s="4"/>
@@ -2946,17 +2946,17 @@
       <c r="W18" s="3"/>
       <c r="X18" s="3"/>
     </row>
-    <row r="19" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="5" t="s">
+    <row r="19" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+      <c r="A19" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="3">
-        <v>1</v>
-      </c>
-      <c r="D19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -2978,20 +2978,26 @@
       <c r="W19" s="3"/>
       <c r="X19" s="3"/>
     </row>
-    <row r="20" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="6" t="s">
-        <v>25</v>
+    <row r="20" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+      <c r="A20" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4" t="s">
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="3">
+        <v>5</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -3010,9 +3016,9 @@
       <c r="W20" s="3"/>
       <c r="X20" s="3"/>
     </row>
-    <row r="21" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A21" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>14</v>
@@ -3020,15 +3026,15 @@
       <c r="C21" s="3">
         <v>1</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E21" s="4"/>
       <c r="F21" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -3048,9 +3054,9 @@
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
     </row>
-    <row r="22" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A22" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>14</v>
@@ -3058,16 +3064,14 @@
       <c r="C22" s="3">
         <v>1</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E22" s="4"/>
       <c r="F22" s="3">
-        <v>6</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>29</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
@@ -3086,9 +3090,9 @@
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
     </row>
-    <row r="23" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A23" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>14</v>
@@ -3096,12 +3100,12 @@
       <c r="C23" s="3">
         <v>1</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E23" s="4"/>
       <c r="F23" s="3">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -3122,9 +3126,9 @@
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
     </row>
-    <row r="24" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A24" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>14</v>
@@ -3132,13 +3136,11 @@
       <c r="C24" s="3">
         <v>1</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E24" s="4"/>
-      <c r="F24" s="3">
-        <v>10</v>
-      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -3158,18 +3160,18 @@
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
     </row>
-    <row r="25" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A25" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="3">
-        <v>1</v>
-      </c>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="4"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -3190,15 +3192,15 @@
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
     </row>
-    <row r="26" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A26" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="3"/>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E26" s="4"/>
@@ -3222,15 +3224,15 @@
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
     </row>
-    <row r="27" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A27" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C27" s="3"/>
-      <c r="D27" s="4" t="s">
+      <c r="D27" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E27" s="4"/>
@@ -3254,15 +3256,15 @@
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
     </row>
-    <row r="28" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C28" s="3"/>
-      <c r="D28" s="4" t="s">
+      <c r="D28" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E28" s="4"/>
@@ -3286,15 +3288,15 @@
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
     </row>
-    <row r="29" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A29" s="5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C29" s="3"/>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E29" s="4"/>
@@ -3318,17 +3320,15 @@
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
     </row>
-    <row r="30" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="5" t="s">
-        <v>38</v>
+    <row r="30" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+      <c r="A30" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="D30" s="26"/>
       <c r="E30" s="4"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -3350,15 +3350,17 @@
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
     </row>
-    <row r="31" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="7" t="s">
-        <v>39</v>
+    <row r="31" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+      <c r="A31" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
+      <c r="D31" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E31" s="4"/>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -3380,15 +3382,15 @@
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
     </row>
-    <row r="32" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A32" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>40</v>
       </c>
       <c r="C32" s="3"/>
-      <c r="D32" s="4" t="s">
+      <c r="D32" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E32" s="4"/>
@@ -3412,20 +3414,24 @@
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
     </row>
-    <row r="33" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C33" s="3">
+        <v>1</v>
+      </c>
+      <c r="D33" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="4"/>
+      <c r="E33" s="3"/>
       <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+      <c r="G33" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3"/>
       <c r="J33" s="3"/>
@@ -3446,7 +3452,7 @@
     </row>
     <row r="34" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A34" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>44</v>
@@ -3460,7 +3466,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
       <c r="G34" s="3" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3"/>
@@ -3482,7 +3488,7 @@
     </row>
     <row r="35" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A35" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>44</v>
@@ -3496,7 +3502,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3"/>
@@ -3518,7 +3524,7 @@
     </row>
     <row r="36" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>44</v>
@@ -3532,7 +3538,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3"/>
@@ -3554,7 +3560,7 @@
     </row>
     <row r="37" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>44</v>
@@ -3590,7 +3596,7 @@
     </row>
     <row r="38" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A38" s="5" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>44</v>
@@ -3603,9 +3609,7 @@
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
-      <c r="G38" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="G38" s="3"/>
       <c r="H38" s="3"/>
       <c r="I38" s="3"/>
       <c r="J38" s="3"/>
@@ -3626,20 +3630,20 @@
     </row>
     <row r="39" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A39" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C39" s="3">
-        <v>1</v>
-      </c>
+      <c r="C39" s="3"/>
       <c r="D39" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E39" s="3"/>
       <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
+      <c r="G39" s="3" t="s">
+        <v>575</v>
+      </c>
       <c r="H39" s="3"/>
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
@@ -3660,7 +3664,7 @@
     </row>
     <row r="40" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A40" s="5" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>44</v>
@@ -3671,9 +3675,7 @@
       </c>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
-      <c r="G40" s="3" t="s">
-        <v>575</v>
-      </c>
+      <c r="G40" s="3"/>
       <c r="H40" s="3"/>
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
@@ -3694,10 +3696,10 @@
     </row>
     <row r="41" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A41" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>44</v>
+        <v>570</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="26" t="s">
@@ -3726,15 +3728,13 @@
     </row>
     <row r="42" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A42" s="5" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>570</v>
+        <v>58</v>
       </c>
       <c r="C42" s="3"/>
-      <c r="D42" s="26" t="s">
-        <v>15</v>
-      </c>
+      <c r="D42" s="26"/>
       <c r="E42" s="3"/>
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
@@ -3756,15 +3756,15 @@
       <c r="W42" s="3"/>
       <c r="X42" s="3"/>
     </row>
-    <row r="43" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A43" s="5" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
+      <c r="D43" s="26"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
@@ -3786,15 +3786,15 @@
       <c r="W43" s="3"/>
       <c r="X43" s="3"/>
     </row>
-    <row r="44" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A44" s="5" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
+      <c r="D44" s="26"/>
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
@@ -3816,15 +3816,15 @@
       <c r="W44" s="3"/>
       <c r="X44" s="3"/>
     </row>
-    <row r="45" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A45" s="5" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
+      <c r="D45" s="26"/>
       <c r="E45" s="3"/>
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
@@ -3846,15 +3846,15 @@
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
     </row>
-    <row r="46" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A46" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
+      <c r="D46" s="26"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
@@ -3876,15 +3876,15 @@
       <c r="W46" s="3"/>
       <c r="X46" s="3"/>
     </row>
-    <row r="47" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A47" s="5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="D47" s="26"/>
       <c r="E47" s="3"/>
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
@@ -3906,15 +3906,15 @@
       <c r="W47" s="3"/>
       <c r="X47" s="3"/>
     </row>
-    <row r="48" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A48" s="5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
+      <c r="D48" s="26"/>
       <c r="E48" s="3"/>
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
@@ -3936,15 +3936,15 @@
       <c r="W48" s="3"/>
       <c r="X48" s="3"/>
     </row>
-    <row r="49" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A49" s="5" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
+      <c r="D49" s="26"/>
       <c r="E49" s="3"/>
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
@@ -3966,15 +3966,15 @@
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
     </row>
-    <row r="50" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A50" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+      <c r="D50" s="26"/>
       <c r="E50" s="3"/>
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
@@ -3996,15 +3996,15 @@
       <c r="W50" s="3"/>
       <c r="X50" s="3"/>
     </row>
-    <row r="51" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A51" s="5" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
+      <c r="D51" s="26"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
@@ -4026,15 +4026,15 @@
       <c r="W51" s="3"/>
       <c r="X51" s="3"/>
     </row>
-    <row r="52" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A52" s="5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C52" s="3"/>
-      <c r="D52" s="3"/>
+      <c r="D52" s="26"/>
       <c r="E52" s="3"/>
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
@@ -4056,15 +4056,15 @@
       <c r="W52" s="3"/>
       <c r="X52" s="3"/>
     </row>
-    <row r="53" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A53" s="5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C53" s="3"/>
-      <c r="D53" s="3"/>
+      <c r="D53" s="26"/>
       <c r="E53" s="3"/>
       <c r="F53" s="3"/>
       <c r="G53" s="3"/>
@@ -4086,15 +4086,15 @@
       <c r="W53" s="3"/>
       <c r="X53" s="3"/>
     </row>
-    <row r="54" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A54" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C54" s="3"/>
-      <c r="D54" s="3"/>
+      <c r="D54" s="26"/>
       <c r="E54" s="3"/>
       <c r="F54" s="3"/>
       <c r="G54" s="3"/>
@@ -4116,15 +4116,15 @@
       <c r="W54" s="3"/>
       <c r="X54" s="3"/>
     </row>
-    <row r="55" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A55" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
+      <c r="D55" s="26"/>
       <c r="E55" s="3"/>
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
@@ -4146,15 +4146,15 @@
       <c r="W55" s="3"/>
       <c r="X55" s="3"/>
     </row>
-    <row r="56" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A56" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
+      <c r="D56" s="26"/>
       <c r="E56" s="3"/>
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
@@ -4176,15 +4176,15 @@
       <c r="W56" s="3"/>
       <c r="X56" s="3"/>
     </row>
-    <row r="57" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A57" s="5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
+      <c r="D57" s="26"/>
       <c r="E57" s="3"/>
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
@@ -4206,15 +4206,15 @@
       <c r="W57" s="3"/>
       <c r="X57" s="3"/>
     </row>
-    <row r="58" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A58" s="5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>58</v>
       </c>
       <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
+      <c r="D58" s="26"/>
       <c r="E58" s="3"/>
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
@@ -4236,15 +4236,15 @@
       <c r="W58" s="3"/>
       <c r="X58" s="3"/>
     </row>
-    <row r="59" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A59" s="5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
+      <c r="D59" s="26"/>
       <c r="E59" s="3"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
@@ -4266,15 +4266,15 @@
       <c r="W59" s="3"/>
       <c r="X59" s="3"/>
     </row>
-    <row r="60" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A60" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C60" s="3"/>
-      <c r="D60" s="3"/>
+      <c r="D60" s="26"/>
       <c r="E60" s="3"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
@@ -4296,15 +4296,15 @@
       <c r="W60" s="3"/>
       <c r="X60" s="3"/>
     </row>
-    <row r="61" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A61" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
+      <c r="D61" s="26"/>
       <c r="E61" s="3"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
@@ -4326,15 +4326,15 @@
       <c r="W61" s="3"/>
       <c r="X61" s="3"/>
     </row>
-    <row r="62" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A62" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
+      <c r="D62" s="26"/>
       <c r="E62" s="3"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
@@ -4356,15 +4356,15 @@
       <c r="W62" s="3"/>
       <c r="X62" s="3"/>
     </row>
-    <row r="63" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A63" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
+      <c r="D63" s="26"/>
       <c r="E63" s="3"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
@@ -4386,15 +4386,15 @@
       <c r="W63" s="3"/>
       <c r="X63" s="3"/>
     </row>
-    <row r="64" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A64" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>78</v>
       </c>
       <c r="C64" s="3"/>
-      <c r="D64" s="3"/>
+      <c r="D64" s="26"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
@@ -4416,15 +4416,15 @@
       <c r="W64" s="3"/>
       <c r="X64" s="3"/>
     </row>
-    <row r="65" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A65" s="5" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
+      <c r="D65" s="26"/>
       <c r="E65" s="3"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
@@ -4446,15 +4446,15 @@
       <c r="W65" s="3"/>
       <c r="X65" s="3"/>
     </row>
-    <row r="66" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A66" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
+      <c r="D66" s="26"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -4476,15 +4476,15 @@
       <c r="W66" s="3"/>
       <c r="X66" s="3"/>
     </row>
-    <row r="67" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A67" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
+      <c r="D67" s="26"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -4506,15 +4506,15 @@
       <c r="W67" s="3"/>
       <c r="X67" s="3"/>
     </row>
-    <row r="68" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A68" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>86</v>
       </c>
       <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
+      <c r="D68" s="26"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -4536,15 +4536,15 @@
       <c r="W68" s="3"/>
       <c r="X68" s="3"/>
     </row>
-    <row r="69" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A69" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
+      <c r="D69" s="26"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -4566,15 +4566,15 @@
       <c r="W69" s="3"/>
       <c r="X69" s="3"/>
     </row>
-    <row r="70" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A70" s="5" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
+      <c r="D70" s="26"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -4596,15 +4596,15 @@
       <c r="W70" s="3"/>
       <c r="X70" s="3"/>
     </row>
-    <row r="71" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A71" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>90</v>
       </c>
       <c r="C71" s="3"/>
-      <c r="D71" s="3"/>
+      <c r="D71" s="26"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>
@@ -4626,15 +4626,15 @@
       <c r="W71" s="3"/>
       <c r="X71" s="3"/>
     </row>
-    <row r="72" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A72" s="5" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="C72" s="3"/>
-      <c r="D72" s="3"/>
+      <c r="D72" s="26"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
       <c r="G72" s="3"/>
@@ -4656,15 +4656,15 @@
       <c r="W72" s="3"/>
       <c r="X72" s="3"/>
     </row>
-    <row r="73" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A73" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C73" s="3"/>
-      <c r="D73" s="3"/>
+      <c r="D73" s="26"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
       <c r="G73" s="3"/>
@@ -4686,18 +4686,22 @@
       <c r="W73" s="3"/>
       <c r="X73" s="3"/>
     </row>
-    <row r="74" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A74" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
+      <c r="D74" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
-      <c r="G74" s="3"/>
+      <c r="G74" s="3" t="s">
+        <v>572</v>
+      </c>
       <c r="H74" s="3"/>
       <c r="I74" s="3"/>
       <c r="J74" s="3"/>
@@ -4716,9 +4720,9 @@
       <c r="W74" s="3"/>
       <c r="X74" s="3"/>
     </row>
-    <row r="75" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A75" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>98</v>
@@ -4750,12 +4754,12 @@
       <c r="W75" s="3"/>
       <c r="X75" s="3"/>
     </row>
-    <row r="76" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A76" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="C76" s="3"/>
       <c r="D76" s="26" t="s">
@@ -4763,9 +4767,7 @@
       </c>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
-      <c r="G76" s="3" t="s">
-        <v>572</v>
-      </c>
+      <c r="G76" s="3"/>
       <c r="H76" s="3"/>
       <c r="I76" s="3"/>
       <c r="J76" s="3"/>
@@ -4784,12 +4786,12 @@
       <c r="W76" s="3"/>
       <c r="X76" s="3"/>
     </row>
-    <row r="77" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A77" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>101</v>
+        <v>573</v>
       </c>
       <c r="C77" s="3"/>
       <c r="D77" s="26" t="s">
@@ -4797,7 +4799,9 @@
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
-      <c r="G77" s="3"/>
+      <c r="G77" s="3" t="s">
+        <v>572</v>
+      </c>
       <c r="H77" s="3"/>
       <c r="I77" s="3"/>
       <c r="J77" s="3"/>
@@ -4818,7 +4822,7 @@
     </row>
     <row r="78" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A78" s="5" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>573</v>
@@ -4850,12 +4854,12 @@
       <c r="W78" s="3"/>
       <c r="X78" s="3"/>
     </row>
-    <row r="79" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A79" s="5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C79" s="3"/>
       <c r="D79" s="26" t="s">
@@ -4884,12 +4888,12 @@
       <c r="W79" s="3"/>
       <c r="X79" s="3"/>
     </row>
-    <row r="80" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A80" s="5" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>574</v>
+        <v>106</v>
       </c>
       <c r="C80" s="3"/>
       <c r="D80" s="26" t="s">
@@ -4897,9 +4901,7 @@
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="3"/>
-      <c r="G80" s="3" t="s">
-        <v>572</v>
-      </c>
+      <c r="G80" s="3"/>
       <c r="H80" s="3"/>
       <c r="I80" s="3"/>
       <c r="J80" s="3"/>
@@ -4918,15 +4920,17 @@
       <c r="W80" s="3"/>
       <c r="X80" s="3"/>
     </row>
-    <row r="81" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A81" s="5" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C81" s="3"/>
-      <c r="D81" s="3"/>
+      <c r="D81" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E81" s="3"/>
       <c r="F81" s="3"/>
       <c r="G81" s="3"/>
@@ -4948,15 +4952,17 @@
       <c r="W81" s="3"/>
       <c r="X81" s="3"/>
     </row>
-    <row r="82" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A82" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C82" s="3"/>
-      <c r="D82" s="3"/>
+      <c r="D82" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E82" s="3"/>
       <c r="F82" s="3"/>
       <c r="G82" s="3"/>
@@ -4978,15 +4984,17 @@
       <c r="W82" s="3"/>
       <c r="X82" s="3"/>
     </row>
-    <row r="83" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A83" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>106</v>
       </c>
       <c r="C83" s="3"/>
-      <c r="D83" s="3"/>
+      <c r="D83" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
       <c r="G83" s="3"/>
@@ -5008,15 +5016,15 @@
       <c r="W83" s="3"/>
       <c r="X83" s="3"/>
     </row>
-    <row r="84" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A84" s="5" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="C84" s="3"/>
-      <c r="D84" s="3"/>
+      <c r="D84" s="26"/>
       <c r="E84" s="3"/>
       <c r="F84" s="3"/>
       <c r="G84" s="3"/>
@@ -5038,15 +5046,15 @@
       <c r="W84" s="3"/>
       <c r="X84" s="3"/>
     </row>
-    <row r="85" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A85" s="5" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C85" s="3"/>
-      <c r="D85" s="3"/>
+      <c r="D85" s="26"/>
       <c r="E85" s="3"/>
       <c r="F85" s="3"/>
       <c r="G85" s="3"/>
@@ -5068,15 +5076,15 @@
       <c r="W85" s="3"/>
       <c r="X85" s="3"/>
     </row>
-    <row r="86" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A86" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C86" s="3"/>
-      <c r="D86" s="3"/>
+      <c r="D86" s="26"/>
       <c r="E86" s="3"/>
       <c r="F86" s="3"/>
       <c r="G86" s="3"/>
@@ -5098,15 +5106,15 @@
       <c r="W86" s="3"/>
       <c r="X86" s="3"/>
     </row>
-    <row r="87" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A87" s="5" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
+      <c r="D87" s="26"/>
       <c r="E87" s="3"/>
       <c r="F87" s="3"/>
       <c r="G87" s="3"/>
@@ -5128,15 +5136,15 @@
       <c r="W87" s="3"/>
       <c r="X87" s="3"/>
     </row>
-    <row r="88" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A88" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>111</v>
       </c>
       <c r="C88" s="3"/>
-      <c r="D88" s="3"/>
+      <c r="D88" s="26"/>
       <c r="E88" s="3"/>
       <c r="F88" s="3"/>
       <c r="G88" s="3"/>
@@ -5158,15 +5166,15 @@
       <c r="W88" s="3"/>
       <c r="X88" s="3"/>
     </row>
-    <row r="89" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A89" s="5" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="C89" s="3"/>
-      <c r="D89" s="3"/>
+      <c r="D89" s="26"/>
       <c r="E89" s="3"/>
       <c r="F89" s="3"/>
       <c r="G89" s="3"/>
@@ -5188,15 +5196,15 @@
       <c r="W89" s="3"/>
       <c r="X89" s="3"/>
     </row>
-    <row r="90" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A90" s="5" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C90" s="3"/>
-      <c r="D90" s="3"/>
+      <c r="D90" s="26"/>
       <c r="E90" s="3"/>
       <c r="F90" s="3"/>
       <c r="G90" s="3"/>
@@ -5218,15 +5226,15 @@
       <c r="W90" s="3"/>
       <c r="X90" s="3"/>
     </row>
-    <row r="91" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A91" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C91" s="3"/>
-      <c r="D91" s="3"/>
+      <c r="D91" s="26"/>
       <c r="E91" s="3"/>
       <c r="F91" s="3"/>
       <c r="G91" s="3"/>
@@ -5248,15 +5256,15 @@
       <c r="W91" s="3"/>
       <c r="X91" s="3"/>
     </row>
-    <row r="92" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A92" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C92" s="3"/>
-      <c r="D92" s="3"/>
+      <c r="D92" s="26"/>
       <c r="E92" s="3"/>
       <c r="F92" s="3"/>
       <c r="G92" s="3"/>
@@ -5278,15 +5286,15 @@
       <c r="W92" s="3"/>
       <c r="X92" s="3"/>
     </row>
-    <row r="93" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A93" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C93" s="3"/>
-      <c r="D93" s="3"/>
+      <c r="D93" s="26"/>
       <c r="E93" s="3"/>
       <c r="F93" s="3"/>
       <c r="G93" s="3"/>
@@ -5308,15 +5316,15 @@
       <c r="W93" s="3"/>
       <c r="X93" s="3"/>
     </row>
-    <row r="94" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A94" s="5" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C94" s="3"/>
-      <c r="D94" s="3"/>
+      <c r="D94" s="26"/>
       <c r="E94" s="3"/>
       <c r="F94" s="3"/>
       <c r="G94" s="3"/>
@@ -5338,15 +5346,15 @@
       <c r="W94" s="3"/>
       <c r="X94" s="3"/>
     </row>
-    <row r="95" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A95" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
+      <c r="D95" s="26"/>
       <c r="E95" s="3"/>
       <c r="F95" s="3"/>
       <c r="G95" s="3"/>
@@ -5368,15 +5376,15 @@
       <c r="W95" s="3"/>
       <c r="X95" s="3"/>
     </row>
-    <row r="96" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A96" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>117</v>
       </c>
       <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
+      <c r="D96" s="26"/>
       <c r="E96" s="3"/>
       <c r="F96" s="3"/>
       <c r="G96" s="3"/>
@@ -5398,16 +5406,20 @@
       <c r="W96" s="3"/>
       <c r="X96" s="3"/>
     </row>
-    <row r="97" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A97" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="3"/>
+        <v>126</v>
+      </c>
+      <c r="C97" s="3">
+        <v>2</v>
+      </c>
+      <c r="D97" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E97" s="4"/>
       <c r="F97" s="3"/>
       <c r="G97" s="3"/>
       <c r="H97" s="3"/>
@@ -5428,9 +5440,9 @@
       <c r="W97" s="3"/>
       <c r="X97" s="3"/>
     </row>
-    <row r="98" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A98" s="5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>126</v>
@@ -5438,7 +5450,7 @@
       <c r="C98" s="3">
         <v>2</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="D98" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E98" s="4"/>
@@ -5462,17 +5474,17 @@
       <c r="W98" s="3"/>
       <c r="X98" s="3"/>
     </row>
-    <row r="99" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A99" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C99" s="3">
-        <v>2</v>
-      </c>
-      <c r="D99" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D99" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E99" s="4"/>
@@ -5496,9 +5508,9 @@
       <c r="W99" s="3"/>
       <c r="X99" s="3"/>
     </row>
-    <row r="100" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A100" s="5" t="s">
-        <v>128</v>
+    <row r="100" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+      <c r="A100" s="25" t="s">
+        <v>129</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>126</v>
@@ -5506,7 +5518,7 @@
       <c r="C100" s="3">
         <v>1</v>
       </c>
-      <c r="D100" s="4" t="s">
+      <c r="D100" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E100" s="4"/>
@@ -5530,17 +5542,17 @@
       <c r="W100" s="3"/>
       <c r="X100" s="3"/>
     </row>
-    <row r="101" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A101" s="25" t="s">
-        <v>129</v>
+    <row r="101" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+      <c r="A101" s="5" t="s">
+        <v>130</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C101" s="3">
-        <v>1</v>
-      </c>
-      <c r="D101" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E101" s="4"/>
@@ -5564,9 +5576,9 @@
       <c r="W101" s="3"/>
       <c r="X101" s="3"/>
     </row>
-    <row r="102" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A102" s="5" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>126</v>
@@ -5574,7 +5586,7 @@
       <c r="C102" s="3">
         <v>2</v>
       </c>
-      <c r="D102" s="4" t="s">
+      <c r="D102" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E102" s="4"/>
@@ -5598,9 +5610,9 @@
       <c r="W102" s="3"/>
       <c r="X102" s="3"/>
     </row>
-    <row r="103" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A103" s="5" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>126</v>
@@ -5608,7 +5620,7 @@
       <c r="C103" s="3">
         <v>2</v>
       </c>
-      <c r="D103" s="4" t="s">
+      <c r="D103" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E103" s="4"/>
@@ -5632,9 +5644,9 @@
       <c r="W103" s="3"/>
       <c r="X103" s="3"/>
     </row>
-    <row r="104" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A104" s="5" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>126</v>
@@ -5642,7 +5654,7 @@
       <c r="C104" s="3">
         <v>2</v>
       </c>
-      <c r="D104" s="4" t="s">
+      <c r="D104" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E104" s="4"/>
@@ -5666,17 +5678,17 @@
       <c r="W104" s="3"/>
       <c r="X104" s="3"/>
     </row>
-    <row r="105" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A105" s="5" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C105" s="3">
-        <v>2</v>
-      </c>
-      <c r="D105" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D105" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E105" s="4"/>
@@ -5700,20 +5712,16 @@
       <c r="W105" s="3"/>
       <c r="X105" s="3"/>
     </row>
-    <row r="106" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A106" s="5" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C106" s="3">
-        <v>1</v>
-      </c>
-      <c r="D106" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E106" s="4"/>
+        <v>136</v>
+      </c>
+      <c r="C106" s="3"/>
+      <c r="D106" s="26"/>
+      <c r="E106" s="3"/>
       <c r="F106" s="3"/>
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
@@ -5736,13 +5744,13 @@
     </row>
     <row r="107" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A107" s="5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>136</v>
       </c>
       <c r="C107" s="3"/>
-      <c r="D107" s="3"/>
+      <c r="D107" s="26"/>
       <c r="E107" s="3"/>
       <c r="F107" s="3"/>
       <c r="G107" s="3"/>
@@ -5766,13 +5774,13 @@
     </row>
     <row r="108" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A108" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B108" s="2" t="s">
         <v>136</v>
       </c>
       <c r="C108" s="3"/>
-      <c r="D108" s="3"/>
+      <c r="D108" s="26"/>
       <c r="E108" s="3"/>
       <c r="F108" s="3"/>
       <c r="G108" s="3"/>
@@ -5796,13 +5804,13 @@
     </row>
     <row r="109" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A109" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C109" s="3"/>
-      <c r="D109" s="3"/>
+      <c r="D109" s="26"/>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
@@ -5824,15 +5832,15 @@
       <c r="W109" s="3"/>
       <c r="X109" s="3"/>
     </row>
-    <row r="110" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A110" s="5" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B110" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C110" s="3"/>
-      <c r="D110" s="3"/>
+      <c r="D110" s="26"/>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
@@ -5854,15 +5862,15 @@
       <c r="W110" s="3"/>
       <c r="X110" s="3"/>
     </row>
-    <row r="111" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A111" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B111" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C111" s="3"/>
-      <c r="D111" s="3"/>
+      <c r="D111" s="26"/>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
@@ -5884,15 +5892,15 @@
       <c r="W111" s="3"/>
       <c r="X111" s="3"/>
     </row>
-    <row r="112" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A112" s="5" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B112" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C112" s="3"/>
-      <c r="D112" s="3"/>
+      <c r="D112" s="26"/>
       <c r="E112" s="3"/>
       <c r="F112" s="3"/>
       <c r="G112" s="3"/>
@@ -5914,15 +5922,15 @@
       <c r="W112" s="3"/>
       <c r="X112" s="3"/>
     </row>
-    <row r="113" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A113" s="5" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B113" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C113" s="3"/>
-      <c r="D113" s="3"/>
+      <c r="D113" s="26"/>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
@@ -5944,15 +5952,15 @@
       <c r="W113" s="3"/>
       <c r="X113" s="3"/>
     </row>
-    <row r="114" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A114" s="5" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B114" s="2" t="s">
         <v>140</v>
       </c>
       <c r="C114" s="3"/>
-      <c r="D114" s="3"/>
+      <c r="D114" s="26"/>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
@@ -5974,16 +5982,20 @@
       <c r="W114" s="3"/>
       <c r="X114" s="3"/>
     </row>
-    <row r="115" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A115" s="5" t="s">
-        <v>145</v>
+    <row r="115" spans="1:24" ht="15" x14ac:dyDescent="0.2">
+      <c r="A115" s="8" t="s">
+        <v>146</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="3"/>
+      <c r="D115" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E115" s="4" t="s">
+        <v>565</v>
+      </c>
       <c r="F115" s="3"/>
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
@@ -6004,15 +6016,15 @@
       <c r="W115" s="3"/>
       <c r="X115" s="3"/>
     </row>
-    <row r="116" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A116" s="8" t="s">
-        <v>146</v>
+        <v>261</v>
       </c>
       <c r="B116" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C116" s="3"/>
-      <c r="D116" s="4" t="s">
+      <c r="D116" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E116" s="4" t="s">
@@ -6038,15 +6050,15 @@
       <c r="W116" s="3"/>
       <c r="X116" s="3"/>
     </row>
-    <row r="117" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A117" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B117" s="2" t="s">
         <v>126</v>
       </c>
       <c r="C117" s="3"/>
-      <c r="D117" s="4" t="s">
+      <c r="D117" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E117" s="4" t="s">
@@ -6072,15 +6084,15 @@
       <c r="W117" s="3"/>
       <c r="X117" s="3"/>
     </row>
-    <row r="118" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A118" s="8" t="s">
-        <v>263</v>
+        <v>197</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="C118" s="3"/>
-      <c r="D118" s="4" t="s">
+      <c r="D118" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E118" s="4" t="s">
@@ -6106,15 +6118,15 @@
       <c r="W118" s="3"/>
       <c r="X118" s="3"/>
     </row>
-    <row r="119" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A119" s="8" t="s">
-        <v>197</v>
+        <v>237</v>
       </c>
       <c r="B119" s="2" t="s">
         <v>158</v>
       </c>
       <c r="C119" s="3"/>
-      <c r="D119" s="4" t="s">
+      <c r="D119" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E119" s="4" t="s">
@@ -6140,20 +6152,18 @@
       <c r="W119" s="3"/>
       <c r="X119" s="3"/>
     </row>
-    <row r="120" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A120" s="8" t="s">
-        <v>237</v>
+        <v>199</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>158</v>
+        <v>566</v>
       </c>
       <c r="C120" s="3"/>
-      <c r="D120" s="4" t="s">
+      <c r="D120" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="E120" s="4" t="s">
-        <v>565</v>
-      </c>
+      <c r="E120" s="4"/>
       <c r="F120" s="3"/>
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
@@ -6174,15 +6184,15 @@
       <c r="W120" s="3"/>
       <c r="X120" s="3"/>
     </row>
-    <row r="121" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A121" s="8" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B121" s="2" t="s">
         <v>566</v>
       </c>
       <c r="C121" s="3"/>
-      <c r="D121" s="4" t="s">
+      <c r="D121" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E121" s="4"/>
@@ -6206,15 +6216,15 @@
       <c r="W121" s="3"/>
       <c r="X121" s="3"/>
     </row>
-    <row r="122" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A122" s="8" t="s">
-        <v>201</v>
+        <v>567</v>
       </c>
       <c r="B122" s="2" t="s">
         <v>566</v>
       </c>
       <c r="C122" s="3"/>
-      <c r="D122" s="4" t="s">
+      <c r="D122" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E122" s="4"/>
@@ -6238,15 +6248,15 @@
       <c r="W122" s="3"/>
       <c r="X122" s="3"/>
     </row>
-    <row r="123" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A123" s="8" t="s">
-        <v>567</v>
+        <v>342</v>
       </c>
       <c r="B123" s="2" t="s">
         <v>566</v>
       </c>
       <c r="C123" s="3"/>
-      <c r="D123" s="4" t="s">
+      <c r="D123" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E123" s="4"/>
@@ -6270,15 +6280,15 @@
       <c r="W123" s="3"/>
       <c r="X123" s="3"/>
     </row>
-    <row r="124" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A124" s="8" t="s">
-        <v>342</v>
+        <v>203</v>
       </c>
       <c r="B124" s="2" t="s">
         <v>566</v>
       </c>
       <c r="C124" s="3"/>
-      <c r="D124" s="4" t="s">
+      <c r="D124" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E124" s="4"/>
@@ -6302,15 +6312,15 @@
       <c r="W124" s="3"/>
       <c r="X124" s="3"/>
     </row>
-    <row r="125" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:24" ht="15" x14ac:dyDescent="0.2">
       <c r="A125" s="8" t="s">
-        <v>203</v>
+        <v>569</v>
       </c>
       <c r="B125" s="2" t="s">
         <v>566</v>
       </c>
       <c r="C125" s="3"/>
-      <c r="D125" s="4" t="s">
+      <c r="D125" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E125" s="4"/>
@@ -6334,15 +6344,15 @@
       <c r="W125" s="3"/>
       <c r="X125" s="3"/>
     </row>
-    <row r="126" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A126" s="8" t="s">
-        <v>569</v>
+    <row r="126" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+      <c r="A126" s="5" t="s">
+        <v>571</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>566</v>
+        <v>101</v>
       </c>
       <c r="C126" s="3"/>
-      <c r="D126" s="4" t="s">
+      <c r="D126" s="26" t="s">
         <v>15</v>
       </c>
       <c r="E126" s="4"/>
@@ -6366,17 +6376,11 @@
       <c r="W126" s="3"/>
       <c r="X126" s="3"/>
     </row>
-    <row r="127" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
-      <c r="A127" s="5" t="s">
-        <v>571</v>
-      </c>
-      <c r="B127" s="2" t="s">
-        <v>101</v>
-      </c>
+    <row r="127" spans="1:24" ht="13" x14ac:dyDescent="0.15">
+      <c r="A127" s="3"/>
+      <c r="B127" s="3"/>
       <c r="C127" s="3"/>
-      <c r="D127" s="26" t="s">
-        <v>15</v>
-      </c>
+      <c r="D127" s="26"/>
       <c r="E127" s="4"/>
       <c r="F127" s="3"/>
       <c r="G127" s="3"/>
@@ -6450,31 +6454,31 @@
       <c r="W129" s="3"/>
       <c r="X129" s="3"/>
     </row>
-    <row r="130" spans="1:24" ht="13" x14ac:dyDescent="0.15">
-      <c r="A130" s="3"/>
-      <c r="B130" s="3"/>
-      <c r="C130" s="3"/>
-      <c r="D130" s="26"/>
-      <c r="E130" s="4"/>
-      <c r="F130" s="3"/>
-      <c r="G130" s="3"/>
-      <c r="H130" s="3"/>
-      <c r="I130" s="3"/>
-      <c r="J130" s="3"/>
-      <c r="K130" s="3"/>
-      <c r="L130" s="3"/>
-      <c r="M130" s="3"/>
-      <c r="N130" s="3"/>
-      <c r="O130" s="3"/>
-      <c r="P130" s="3"/>
-      <c r="Q130" s="3"/>
-      <c r="R130" s="3"/>
-      <c r="S130" s="3"/>
-      <c r="T130" s="3"/>
-      <c r="U130" s="3"/>
-      <c r="V130" s="3"/>
-      <c r="W130" s="3"/>
-      <c r="X130" s="3"/>
+    <row r="131" spans="1:24" ht="13" x14ac:dyDescent="0.15">
+      <c r="A131" s="3"/>
+      <c r="B131" s="3"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="26"/>
+      <c r="E131" s="4"/>
+      <c r="F131" s="3"/>
+      <c r="G131" s="3"/>
+      <c r="H131" s="3"/>
+      <c r="I131" s="3"/>
+      <c r="J131" s="3"/>
+      <c r="K131" s="3"/>
+      <c r="L131" s="3"/>
+      <c r="M131" s="3"/>
+      <c r="N131" s="3"/>
+      <c r="O131" s="3"/>
+      <c r="P131" s="3"/>
+      <c r="Q131" s="3"/>
+      <c r="R131" s="3"/>
+      <c r="S131" s="3"/>
+      <c r="T131" s="3"/>
+      <c r="U131" s="3"/>
+      <c r="V131" s="3"/>
+      <c r="W131" s="3"/>
+      <c r="X131" s="3"/>
     </row>
     <row r="132" spans="1:24" ht="13" x14ac:dyDescent="0.15">
       <c r="A132" s="3"/>
@@ -6767,7 +6771,7 @@
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
       <c r="D143" s="26"/>
-      <c r="E143" s="4"/>
+      <c r="E143" s="26"/>
       <c r="F143" s="3"/>
       <c r="G143" s="3"/>
       <c r="H143" s="3"/>
@@ -6793,7 +6797,7 @@
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
       <c r="D144" s="26"/>
-      <c r="E144" s="26"/>
+      <c r="E144" s="4"/>
       <c r="F144" s="3"/>
       <c r="G144" s="3"/>
       <c r="H144" s="3"/>
@@ -29096,43 +29100,8 @@
       <c r="W1001" s="3"/>
       <c r="X1001" s="3"/>
     </row>
-    <row r="1002" spans="1:24" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1002" s="3"/>
-      <c r="B1002" s="3"/>
-      <c r="C1002" s="3"/>
-      <c r="D1002" s="26"/>
-      <c r="E1002" s="4"/>
-      <c r="F1002" s="3"/>
-      <c r="G1002" s="3"/>
-      <c r="H1002" s="3"/>
-      <c r="I1002" s="3"/>
-      <c r="J1002" s="3"/>
-      <c r="K1002" s="3"/>
-      <c r="L1002" s="3"/>
-      <c r="M1002" s="3"/>
-      <c r="N1002" s="3"/>
-      <c r="O1002" s="3"/>
-      <c r="P1002" s="3"/>
-      <c r="Q1002" s="3"/>
-      <c r="R1002" s="3"/>
-      <c r="S1002" s="3"/>
-      <c r="T1002" s="3"/>
-      <c r="U1002" s="3"/>
-      <c r="V1002" s="3"/>
-      <c r="W1002" s="3"/>
-      <c r="X1002" s="3"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G127" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Binary Search"/>
-        <filter val="Binary Search / Heap"/>
-        <filter val="Binary Search / Heap / Quick Select"/>
-        <filter val="Trie"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G126" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="A3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -29150,116 +29119,115 @@
     <hyperlink ref="A16" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
     <hyperlink ref="A17" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
     <hyperlink ref="A18" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="A19" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="A21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="A22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="A23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="A24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="A25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="A26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="A27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="A28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="A29" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
-    <hyperlink ref="A30" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="A31" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="A32" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="A33" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="A34" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="A35" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="A36" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="A37" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
-    <hyperlink ref="A38" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="A39" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="A40" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="A41" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="A42" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="A43" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="A44" r:id="rId41" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="A45" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="A46" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="A47" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="A48" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="A49" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="A50" r:id="rId47" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="A51" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="A52" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="A53" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
-    <hyperlink ref="A54" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
-    <hyperlink ref="A55" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="A56" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="A57" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="A58" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="A59" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="A60" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="A61" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="A62" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="A63" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="A64" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="A65" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="A66" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="A67" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="A68" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="A69" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="A70" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="A71" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="A72" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="A73" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="A74" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="A75" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="A76" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="A77" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="A78" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="A79" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="A80" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="A81" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="A82" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="A83" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="A84" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="A85" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="A86" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="A87" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="A88" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="A89" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="A90" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="A91" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="A92" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="A93" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="A94" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="A95" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="A96" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="A97" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
-    <hyperlink ref="A98" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
-    <hyperlink ref="A99" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
-    <hyperlink ref="A100" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
-    <hyperlink ref="A101" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
-    <hyperlink ref="A102" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
-    <hyperlink ref="A103" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
-    <hyperlink ref="A104" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
-    <hyperlink ref="A105" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
-    <hyperlink ref="A106" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
-    <hyperlink ref="A107" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
-    <hyperlink ref="A108" r:id="rId105" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
-    <hyperlink ref="A109" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
-    <hyperlink ref="A110" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
-    <hyperlink ref="A111" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
-    <hyperlink ref="A112" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
-    <hyperlink ref="A113" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
-    <hyperlink ref="A114" r:id="rId111" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
-    <hyperlink ref="A115" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
-    <hyperlink ref="A116" r:id="rId113" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
-    <hyperlink ref="A117" r:id="rId114" display="https://leetcode.com/problems/insert-into-a-binary-search-tree/" xr:uid="{ADBD6DE6-6F81-E641-B4B7-49FE47004641}"/>
-    <hyperlink ref="A118" r:id="rId115" display="https://leetcode.com/problems/delete-node-in-a-bst/" xr:uid="{B1461033-5BA0-7547-925B-C6D108E9EC86}"/>
-    <hyperlink ref="A119" r:id="rId116" display="https://leetcode.com/problems/min-stack/" xr:uid="{D9CEA329-85AD-7145-A930-4573E2655FE5}"/>
-    <hyperlink ref="A120" r:id="rId117" display="https://leetcode.com/problems/evaluate-reverse-polish-notation/" xr:uid="{EE2700FD-DCE0-A541-95CD-CFA938FF0EB1}"/>
-    <hyperlink ref="A121" r:id="rId118" display="https://leetcode.com/problems/daily-temperatures/" xr:uid="{EAEFC768-DCE3-9548-ADC0-421667439610}"/>
-    <hyperlink ref="A122" r:id="rId119" display="https://leetcode.com/problems/buildings-with-an-ocean-view/" xr:uid="{5DCB413A-C4EE-D840-9910-3CB1E3BCBA59}"/>
-    <hyperlink ref="A123" r:id="rId120" display="https://leetcode.com/problems/next-greater-element-i/" xr:uid="{F91D423E-F23F-6544-ACF4-66573BC73611}"/>
-    <hyperlink ref="A124" r:id="rId121" display="https://leetcode.com/problems/132-pattern/" xr:uid="{7C06CC5A-E5D3-C840-BF03-372AE5318481}"/>
-    <hyperlink ref="A125" r:id="rId122" display="https://leetcode.com/problems/remove-k-digits/" xr:uid="{AA5738CB-9E06-E148-A2B3-CF1C00F95632}"/>
-    <hyperlink ref="A15" r:id="rId123" xr:uid="{C9B02FA7-A460-534B-8224-B58EACA416DC}"/>
-    <hyperlink ref="A20" r:id="rId124" xr:uid="{F0DF8437-0D5C-CB47-8F51-866DA9879A59}"/>
-    <hyperlink ref="A126" r:id="rId125" xr:uid="{6D685952-267C-C741-9BCC-8B81CDFEDCF1}"/>
-    <hyperlink ref="A127" r:id="rId126" display="https://leetcode.com/problems/kth-largest-element-in-a-stream/" xr:uid="{332AD428-BEFD-014F-9AF1-BD436C768081}"/>
+    <hyperlink ref="A20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="A22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="A23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="A24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="A25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="A26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="A27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="A28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="A29" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="A30" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="A31" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="A32" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="A33" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="A34" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="A35" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="A36" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="A37" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="A38" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="A39" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="A40" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="A41" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="A42" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="A43" r:id="rId40" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="A44" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="A45" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="A46" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="A47" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="A48" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="A49" r:id="rId46" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="A50" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="A51" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="A52" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000032000000}"/>
+    <hyperlink ref="A53" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000033000000}"/>
+    <hyperlink ref="A54" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="A55" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="A56" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="A57" r:id="rId54" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="A58" r:id="rId55" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="A59" r:id="rId56" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="A60" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="A61" r:id="rId58" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="A62" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="A63" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="A64" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
+    <hyperlink ref="A65" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="A66" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="A67" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="A68" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="A69" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="A70" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="A71" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="A72" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="A73" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="A74" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="A75" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="A76" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="A77" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="A78" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="A79" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="A80" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="A81" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="A82" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="A83" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="A84" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="A85" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="A86" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="A87" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="A88" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="A89" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="A90" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="A91" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="A92" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="A93" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="A94" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="A95" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="A96" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="A97" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005F000000}"/>
+    <hyperlink ref="A98" r:id="rId95" xr:uid="{00000000-0004-0000-0000-000060000000}"/>
+    <hyperlink ref="A99" r:id="rId96" xr:uid="{00000000-0004-0000-0000-000061000000}"/>
+    <hyperlink ref="A100" r:id="rId97" xr:uid="{00000000-0004-0000-0000-000062000000}"/>
+    <hyperlink ref="A101" r:id="rId98" xr:uid="{00000000-0004-0000-0000-000063000000}"/>
+    <hyperlink ref="A102" r:id="rId99" xr:uid="{00000000-0004-0000-0000-000064000000}"/>
+    <hyperlink ref="A103" r:id="rId100" xr:uid="{00000000-0004-0000-0000-000065000000}"/>
+    <hyperlink ref="A104" r:id="rId101" xr:uid="{00000000-0004-0000-0000-000066000000}"/>
+    <hyperlink ref="A105" r:id="rId102" xr:uid="{00000000-0004-0000-0000-000067000000}"/>
+    <hyperlink ref="A106" r:id="rId103" xr:uid="{00000000-0004-0000-0000-000068000000}"/>
+    <hyperlink ref="A107" r:id="rId104" xr:uid="{00000000-0004-0000-0000-000069000000}"/>
+    <hyperlink ref="A108" r:id="rId105" xr:uid="{00000000-0004-0000-0000-00006A000000}"/>
+    <hyperlink ref="A109" r:id="rId106" xr:uid="{00000000-0004-0000-0000-00006B000000}"/>
+    <hyperlink ref="A110" r:id="rId107" xr:uid="{00000000-0004-0000-0000-00006C000000}"/>
+    <hyperlink ref="A111" r:id="rId108" xr:uid="{00000000-0004-0000-0000-00006D000000}"/>
+    <hyperlink ref="A112" r:id="rId109" xr:uid="{00000000-0004-0000-0000-00006E000000}"/>
+    <hyperlink ref="A113" r:id="rId110" xr:uid="{00000000-0004-0000-0000-00006F000000}"/>
+    <hyperlink ref="A114" r:id="rId111" xr:uid="{00000000-0004-0000-0000-000070000000}"/>
+    <hyperlink ref="A115" r:id="rId112" xr:uid="{00000000-0004-0000-0000-000071000000}"/>
+    <hyperlink ref="A116" r:id="rId113" display="https://leetcode.com/problems/insert-into-a-binary-search-tree/" xr:uid="{ADBD6DE6-6F81-E641-B4B7-49FE47004641}"/>
+    <hyperlink ref="A117" r:id="rId114" display="https://leetcode.com/problems/delete-node-in-a-bst/" xr:uid="{B1461033-5BA0-7547-925B-C6D108E9EC86}"/>
+    <hyperlink ref="A118" r:id="rId115" display="https://leetcode.com/problems/min-stack/" xr:uid="{D9CEA329-85AD-7145-A930-4573E2655FE5}"/>
+    <hyperlink ref="A119" r:id="rId116" display="https://leetcode.com/problems/evaluate-reverse-polish-notation/" xr:uid="{EE2700FD-DCE0-A541-95CD-CFA938FF0EB1}"/>
+    <hyperlink ref="A120" r:id="rId117" display="https://leetcode.com/problems/daily-temperatures/" xr:uid="{EAEFC768-DCE3-9548-ADC0-421667439610}"/>
+    <hyperlink ref="A121" r:id="rId118" display="https://leetcode.com/problems/buildings-with-an-ocean-view/" xr:uid="{5DCB413A-C4EE-D840-9910-3CB1E3BCBA59}"/>
+    <hyperlink ref="A122" r:id="rId119" display="https://leetcode.com/problems/next-greater-element-i/" xr:uid="{F91D423E-F23F-6544-ACF4-66573BC73611}"/>
+    <hyperlink ref="A123" r:id="rId120" display="https://leetcode.com/problems/132-pattern/" xr:uid="{7C06CC5A-E5D3-C840-BF03-372AE5318481}"/>
+    <hyperlink ref="A124" r:id="rId121" display="https://leetcode.com/problems/remove-k-digits/" xr:uid="{AA5738CB-9E06-E148-A2B3-CF1C00F95632}"/>
+    <hyperlink ref="A15" r:id="rId122" xr:uid="{C9B02FA7-A460-534B-8224-B58EACA416DC}"/>
+    <hyperlink ref="A19" r:id="rId123" xr:uid="{F0DF8437-0D5C-CB47-8F51-866DA9879A59}"/>
+    <hyperlink ref="A125" r:id="rId124" xr:uid="{6D685952-267C-C741-9BCC-8B81CDFEDCF1}"/>
+    <hyperlink ref="A126" r:id="rId125" display="https://leetcode.com/problems/kth-largest-element-in-a-stream/" xr:uid="{332AD428-BEFD-014F-9AF1-BD436C768081}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -29448,7 +29416,7 @@
   </sheetPr>
   <dimension ref="A1:AB896"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A99" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>

<commit_message>
Add Two Pointers notes
</commit_message>
<xml_diff>
--- a/LEET_CODE_LIST.xlsx
+++ b/LEET_CODE_LIST.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkat/Desktop/DSA_08_29_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2245976-254B-9943-8913-23B29904F03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF1A7B1-D9DD-0C43-9280-12A54013AF5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'amazon 1M'!$A$1:$B$43</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Patterns'!$A$1:$G$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'LeetCode Patterns'!$A$1:$G$129</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'My Patterns'!$A$1:$F$233</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1304" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="596">
   <si>
     <t>Problem Name</t>
   </si>
@@ -2448,7 +2448,7 @@
   <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F111" sqref="F111"/>
+      <selection activeCell="F93" sqref="F93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2493,7 +2493,7 @@
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
     </row>
-    <row r="2" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
@@ -2525,7 +2525,7 @@
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
     </row>
-    <row r="3" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -2557,7 +2557,7 @@
       <c r="W3" s="3"/>
       <c r="X3" s="3"/>
     </row>
-    <row r="4" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -2589,7 +2589,7 @@
       <c r="W4" s="3"/>
       <c r="X4" s="3"/>
     </row>
-    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
@@ -2681,7 +2681,7 @@
       <c r="W7" s="3"/>
       <c r="X7" s="3"/>
     </row>
-    <row r="8" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
@@ -5933,7 +5933,7 @@
       <c r="W108" s="3"/>
       <c r="X108" s="3"/>
     </row>
-    <row r="109" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A109" s="5" t="s">
         <v>139</v>
       </c>
@@ -5941,7 +5941,9 @@
         <v>140</v>
       </c>
       <c r="C109" s="3"/>
-      <c r="D109" s="26"/>
+      <c r="D109" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E109" s="3"/>
       <c r="F109" s="3"/>
       <c r="G109" s="3"/>
@@ -5963,7 +5965,7 @@
       <c r="W109" s="3"/>
       <c r="X109" s="3"/>
     </row>
-    <row r="110" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A110" s="5" t="s">
         <v>141</v>
       </c>
@@ -5971,7 +5973,9 @@
         <v>140</v>
       </c>
       <c r="C110" s="3"/>
-      <c r="D110" s="26"/>
+      <c r="D110" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E110" s="3"/>
       <c r="F110" s="3"/>
       <c r="G110" s="3"/>
@@ -5993,7 +5997,7 @@
       <c r="W110" s="3"/>
       <c r="X110" s="3"/>
     </row>
-    <row r="111" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A111" s="5" t="s">
         <v>142</v>
       </c>
@@ -6001,7 +6005,9 @@
         <v>140</v>
       </c>
       <c r="C111" s="3"/>
-      <c r="D111" s="26"/>
+      <c r="D111" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E111" s="3"/>
       <c r="F111" s="3"/>
       <c r="G111" s="3"/>
@@ -6023,7 +6029,7 @@
       <c r="W111" s="3"/>
       <c r="X111" s="3"/>
     </row>
-    <row r="112" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A112" s="5" t="s">
         <v>143</v>
       </c>
@@ -6055,7 +6061,7 @@
       <c r="W112" s="3"/>
       <c r="X112" s="3"/>
     </row>
-    <row r="113" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A113" s="5" t="s">
         <v>144</v>
       </c>
@@ -6063,7 +6069,9 @@
         <v>140</v>
       </c>
       <c r="C113" s="3"/>
-      <c r="D113" s="26"/>
+      <c r="D113" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E113" s="3"/>
       <c r="F113" s="3"/>
       <c r="G113" s="3"/>
@@ -6085,7 +6093,7 @@
       <c r="W113" s="3"/>
       <c r="X113" s="3"/>
     </row>
-    <row r="114" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A114" s="5" t="s">
         <v>145</v>
       </c>
@@ -6093,7 +6101,9 @@
         <v>140</v>
       </c>
       <c r="C114" s="3"/>
-      <c r="D114" s="26"/>
+      <c r="D114" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E114" s="3"/>
       <c r="F114" s="3"/>
       <c r="G114" s="3"/>
@@ -6509,7 +6519,7 @@
       <c r="W126" s="3"/>
       <c r="X126" s="3"/>
     </row>
-    <row r="127" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A127" s="5" t="s">
         <v>331</v>
       </c>
@@ -6541,7 +6551,7 @@
       <c r="W127" s="3"/>
       <c r="X127" s="3"/>
     </row>
-    <row r="128" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A128" s="5" t="s">
         <v>594</v>
       </c>
@@ -6573,7 +6583,7 @@
       <c r="W128" s="3"/>
       <c r="X128" s="3"/>
     </row>
-    <row r="129" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:24" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A129" s="5" t="s">
         <v>322</v>
       </c>
@@ -29231,16 +29241,17 @@
       <c r="X1000" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G126" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A1:G129" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Array"/>
         <filter val="Arrays"/>
         <filter val="Intervals"/>
         <filter val="Sliding Window"/>
         <filter val="Trie"/>
-        <filter val="Two Pointers"/>
       </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <hyperlinks>

</xml_diff>

<commit_message>
Update Graph Notes and Add Graphs Leetcode
</commit_message>
<xml_diff>
--- a/LEET_CODE_LIST.xlsx
+++ b/LEET_CODE_LIST.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/venkat/Desktop/DSA_08_29_2025/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9773722-1FB7-2E49-AA28-BD63E429C148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B592829-BC13-AA45-96A4-4F4BC52C46E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30240" yWindow="6740" windowWidth="30240" windowHeight="17100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30240" yWindow="6720" windowWidth="30240" windowHeight="18900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LeetCode Patterns" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1377" uniqueCount="608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="609">
   <si>
     <t>Problem Name</t>
   </si>
@@ -1969,6 +1969,9 @@
   </si>
   <si>
     <t>AMD</t>
+  </si>
+  <si>
+    <t>BFSDFS/Graphs</t>
   </si>
 </sst>
 </file>
@@ -2484,7 +2487,7 @@
   <dimension ref="A1:X1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+      <selection activeCell="C141" sqref="C141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3477,15 +3480,17 @@
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
     </row>
-    <row r="30" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
         <v>39</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>40</v>
+        <v>608</v>
       </c>
       <c r="C30" s="3"/>
-      <c r="D30" s="26"/>
+      <c r="D30" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E30" s="4"/>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -4583,7 +4588,7 @@
       <c r="W64" s="3"/>
       <c r="X64" s="3"/>
     </row>
-    <row r="65" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A65" s="5" t="s">
         <v>83</v>
       </c>
@@ -4613,7 +4618,7 @@
       <c r="W65" s="3"/>
       <c r="X65" s="3"/>
     </row>
-    <row r="66" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A66" s="5" t="s">
         <v>85</v>
       </c>
@@ -4621,7 +4626,9 @@
         <v>86</v>
       </c>
       <c r="C66" s="3"/>
-      <c r="D66" s="26"/>
+      <c r="D66" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -4643,7 +4650,7 @@
       <c r="W66" s="3"/>
       <c r="X66" s="3"/>
     </row>
-    <row r="67" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A67" s="5" t="s">
         <v>87</v>
       </c>
@@ -4673,7 +4680,7 @@
       <c r="W67" s="3"/>
       <c r="X67" s="3"/>
     </row>
-    <row r="68" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A68" s="5" t="s">
         <v>88</v>
       </c>
@@ -4681,7 +4688,9 @@
         <v>86</v>
       </c>
       <c r="C68" s="3"/>
-      <c r="D68" s="26"/>
+      <c r="D68" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -4703,7 +4712,7 @@
       <c r="W68" s="3"/>
       <c r="X68" s="3"/>
     </row>
-    <row r="69" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A69" s="5" t="s">
         <v>89</v>
       </c>
@@ -4711,7 +4720,9 @@
         <v>90</v>
       </c>
       <c r="C69" s="3"/>
-      <c r="D69" s="26"/>
+      <c r="D69" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -4733,7 +4744,7 @@
       <c r="W69" s="3"/>
       <c r="X69" s="3"/>
     </row>
-    <row r="70" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A70" s="5" t="s">
         <v>91</v>
       </c>
@@ -4741,7 +4752,9 @@
         <v>90</v>
       </c>
       <c r="C70" s="3"/>
-      <c r="D70" s="26"/>
+      <c r="D70" s="26" t="s">
+        <v>15</v>
+      </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -4763,7 +4776,7 @@
       <c r="W70" s="3"/>
       <c r="X70" s="3"/>
     </row>
-    <row r="71" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A71" s="5" t="s">
         <v>92</v>
       </c>
@@ -4793,7 +4806,7 @@
       <c r="W71" s="3"/>
       <c r="X71" s="3"/>
     </row>
-    <row r="72" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:24" ht="15" x14ac:dyDescent="0.15">
       <c r="A72" s="5" t="s">
         <v>93</v>
       </c>
@@ -4953,7 +4966,7 @@
       <c r="W76" s="3"/>
       <c r="X76" s="3"/>
     </row>
-    <row r="77" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A77" s="5" t="s">
         <v>102</v>
       </c>
@@ -4987,7 +5000,7 @@
       <c r="W77" s="3"/>
       <c r="X77" s="3"/>
     </row>
-    <row r="78" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A78" s="5" t="s">
         <v>103</v>
       </c>
@@ -5906,7 +5919,7 @@
       <c r="W105" s="3"/>
       <c r="X105" s="3"/>
     </row>
-    <row r="106" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A106" s="5" t="s">
         <v>135</v>
       </c>
@@ -5938,7 +5951,7 @@
       <c r="W106" s="3"/>
       <c r="X106" s="3"/>
     </row>
-    <row r="107" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A107" s="5" t="s">
         <v>260</v>
       </c>
@@ -5970,7 +5983,7 @@
       <c r="W107" s="3"/>
       <c r="X107" s="3"/>
     </row>
-    <row r="108" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A108" s="5" t="s">
         <v>137</v>
       </c>
@@ -6002,7 +6015,7 @@
       <c r="W108" s="3"/>
       <c r="X108" s="3"/>
     </row>
-    <row r="109" spans="1:24" ht="15" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:24" ht="15" hidden="1" x14ac:dyDescent="0.15">
       <c r="A109" s="5" t="s">
         <v>138</v>
       </c>
@@ -29343,8 +29356,11 @@
   <autoFilter ref="A1:G130" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Heap / Quick Select"/>
-        <filter val="Trie"/>
+        <filter val="BFSDFS/Graphs"/>
+        <filter val="Graph"/>
+        <filter val="Graph - Union Find"/>
+        <filter val="Graphs"/>
+        <filter val="GraphTopological Sort"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>